<commit_message>
Spring 10: HU1: Diseño de base de datos
</commit_message>
<xml_diff>
--- a/CRONOGRAMA/Actividades por Historia de Usuario.xlsx
+++ b/CRONOGRAMA/Actividades por Historia de Usuario.xlsx
@@ -386,7 +386,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +421,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF158466"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -465,64 +471,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,7 +638,7 @@
       <rgbColor rgb="FFF4CCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFBBC04"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -831,7 +841,7 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1106,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="2" t="n">
         <f aca="false">SUM(C2:C24)</f>
         <v>62.5</v>
       </c>
@@ -1125,7 +1135,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="6"/>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="2" t="n">
         <f aca="false">C25*C26</f>
         <v>400</v>
       </c>
@@ -1135,7 +1145,7 @@
         <v>33</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="2" t="n">
         <f aca="false">C27/40</f>
         <v>10</v>
       </c>
@@ -1167,13 +1177,13 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="67.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,18 +1207,18 @@
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="11" t="str">
+      <c r="B2" s="10" t="str">
         <f aca="false">Epicas!A2</f>
         <v>HU1</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="10" t="n">
         <f aca="false">C2*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1216,223 +1226,223 @@
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="11" t="str">
+      <c r="B3" s="10" t="str">
         <f aca="false">Epicas!A2</f>
         <v>HU1</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="10" t="n">
         <f aca="false">C3*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="11" t="str">
+      <c r="B4" s="10" t="str">
         <f aca="false">Epicas!A2</f>
         <v>HU1</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="10" t="n">
         <f aca="false">C4*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="11" t="str">
+      <c r="B5" s="10" t="str">
         <f aca="false">Epicas!A2</f>
         <v>HU1</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="10" t="n">
         <f aca="false">C5*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="10" t="str">
         <f aca="false">Epicas!A3</f>
         <v>HU2</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="10" t="n">
         <f aca="false">C6*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="11" t="str">
+      <c r="B7" s="10" t="str">
         <f aca="false">Epicas!A3</f>
         <v>HU2</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="10" t="n">
         <f aca="false">C7*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="7" t="str">
+      <c r="B8" s="12" t="str">
         <f aca="false">Epicas!A4</f>
         <v>HU3</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="n">
+      <c r="C8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12" t="n">
         <f aca="false">C8*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="7" t="str">
+      <c r="B9" s="12" t="str">
         <f aca="false">Epicas!A4</f>
         <v>HU3</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="12" t="n">
         <f aca="false">C9*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="7" t="str">
+      <c r="B10" s="2" t="str">
         <f aca="false">Epicas!A5</f>
         <v>HU4</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="2" t="n">
         <f aca="false">C10*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="7" t="str">
+      <c r="B11" s="12" t="str">
         <f aca="false">Epicas!A5</f>
         <v>HU4</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="12" t="n">
         <f aca="false">C11*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="7" t="str">
+      <c r="B12" s="12" t="str">
         <f aca="false">Epicas!A5</f>
         <v>HU4</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7" t="n">
+      <c r="C12" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12" t="n">
         <f aca="false">C12*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="12" t="n">
         <f aca="false">C13*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="n">
+      <c r="C14" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12" t="n">
         <f aca="false">C14*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="n">
+      <c r="C15" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12" t="n">
         <f aca="false">C15*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -1444,11 +1454,11 @@
       <c r="C16" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">C16*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1462,43 +1472,43 @@
       <c r="C17" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">C17*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="12" t="n">
         <f aca="false">C18*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7" t="n">
+      <c r="C19" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12" t="n">
         <f aca="false">C19*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1512,11 +1522,11 @@
       <c r="C20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="2" t="n">
         <f aca="false">C20*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -1528,43 +1538,43 @@
       <c r="C21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="2" t="n">
         <f aca="false">C21*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7" t="n">
+      <c r="C22" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12" t="n">
         <f aca="false">C22*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7" t="n">
+      <c r="C23" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12" t="n">
         <f aca="false">C23*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -1576,11 +1586,11 @@
       <c r="C24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="2" t="n">
         <f aca="false">C24*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1594,43 +1604,43 @@
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D25" s="2" t="n">
         <f aca="false">C25*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7" t="n">
+      <c r="C26" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12" t="n">
         <f aca="false">C26*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="12" t="n">
         <f aca="false">C27*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
@@ -1642,159 +1652,159 @@
       <c r="C28" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="7" t="n">
+      <c r="D28" s="2" t="n">
         <f aca="false">C28*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="12" t="n">
         <f aca="false">C29*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="7" t="n">
+      <c r="C30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="12" t="n">
         <f aca="false">C30*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7" t="n">
+      <c r="C31" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12" t="n">
         <f aca="false">C31*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="C32" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D32" s="7" t="n">
+      <c r="D32" s="12" t="n">
         <f aca="false">C32*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7" t="n">
+      <c r="C33" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="12" t="n">
         <f aca="false">C33*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D34" s="7" t="n">
+      <c r="D34" s="12" t="n">
         <f aca="false">C34*Epicas!$C$26</f>
         <v>9.6</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="35" s="13" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="7" t="n">
+      <c r="C35" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="12" t="n">
         <f aca="false">C35*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" s="13" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" s="7" t="n">
+      <c r="C36" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="12" t="n">
         <f aca="false">C36*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" s="13" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="7" t="n">
+      <c r="C37" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="12" t="n">
         <f aca="false">C37*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
@@ -1806,45 +1816,45 @@
       <c r="C38" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="D38" s="7" t="n">
+      <c r="D38" s="2" t="n">
         <f aca="false">C38*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="C39" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D39" s="7" t="n">
+      <c r="D39" s="12" t="n">
         <f aca="false">C39*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D40" s="7" t="n">
+      <c r="D40" s="12" t="n">
         <f aca="false">C40*Epicas!$C$26</f>
         <v>9.6</v>
       </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
@@ -1856,11 +1866,11 @@
       <c r="C41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D41" s="7" t="n">
+      <c r="D41" s="2" t="n">
         <f aca="false">C41*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E41" s="12"/>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
@@ -1872,11 +1882,11 @@
       <c r="C42" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="D42" s="7" t="n">
+      <c r="D42" s="2" t="n">
         <f aca="false">C42*Epicas!$C$26</f>
         <v>3.2</v>
       </c>
-      <c r="E42" s="12"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
@@ -1888,11 +1898,11 @@
       <c r="C43" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D43" s="7" t="n">
+      <c r="D43" s="2" t="n">
         <f aca="false">C43*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1906,27 +1916,27 @@
       <c r="C44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="7" t="n">
+      <c r="D44" s="2" t="n">
         <f aca="false">C44*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" s="7" t="n">
+      <c r="C45" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="12" t="n">
         <f aca="false">C45*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
@@ -1938,11 +1948,11 @@
       <c r="C46" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D46" s="7" t="n">
+      <c r="D46" s="2" t="n">
         <f aca="false">C46*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E46" s="12"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
@@ -1954,11 +1964,11 @@
       <c r="C47" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D47" s="7" t="n">
+      <c r="D47" s="2" t="n">
         <f aca="false">C47*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="11" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1972,11 +1982,11 @@
       <c r="C48" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D48" s="7" t="n">
+      <c r="D48" s="2" t="n">
         <f aca="false">C48*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E48" s="12"/>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
@@ -1988,11 +1998,11 @@
       <c r="C49" s="2" t="n">
         <v>1.5</v>
       </c>
-      <c r="D49" s="7" t="n">
+      <c r="D49" s="2" t="n">
         <f aca="false">C49*Epicas!$C$26</f>
         <v>9.6</v>
       </c>
-      <c r="E49" s="12"/>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
@@ -2004,11 +2014,11 @@
       <c r="C50" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D50" s="7" t="n">
+      <c r="D50" s="2" t="n">
         <f aca="false">C50*Epicas!$C$26</f>
         <v>19.2</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="11" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2022,11 +2032,11 @@
       <c r="C51" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D51" s="7" t="n">
+      <c r="D51" s="2" t="n">
         <f aca="false">C51*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E51" s="12"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
@@ -2038,11 +2048,11 @@
       <c r="C52" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D52" s="7" t="n">
+      <c r="D52" s="2" t="n">
         <f aca="false">C52*Epicas!$C$26</f>
         <v>12.8</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="11" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2056,18 +2066,18 @@
       <c r="C53" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D53" s="7" t="n">
+      <c r="D53" s="2" t="n">
         <f aca="false">C53*Epicas!$C$26</f>
         <v>6.4</v>
       </c>
-      <c r="E53" s="12"/>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="13" t="n">
+      <c r="D54" s="14" t="n">
         <f aca="false">SUM(D2:D53)</f>
         <v>400</v>
       </c>
-      <c r="E54" s="14"/>
+      <c r="E54" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>